<commit_message>
Distinguished phenotype growth rates ; Acetate media simulation
</commit_message>
<xml_diff>
--- a/CommunityModeling/CommFitting/data/Jeffs_data/Met Model Data Key.xlsx
+++ b/CommunityModeling/CommFitting/data/Jeffs_data/Met Model Data Key.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="65">
   <si>
     <t>Shorthand</t>
   </si>
@@ -214,6 +214,51 @@
   </si>
   <si>
     <t>Acetate at different concentrations</t>
+  </si>
+  <si>
+    <t>Ace KO e coli only</t>
+  </si>
+  <si>
+    <t>Acetate KO Ecoli only 10-21-22</t>
+  </si>
+  <si>
+    <t>https://anl.box.com/s/8lzgu1nf5xaduhldkfafwjpzcwtrhrxt</t>
+  </si>
+  <si>
+    <t>Maltose with acetate at various concentrations</t>
+  </si>
+  <si>
+    <t>Metabolomics</t>
+  </si>
+  <si>
+    <t>8-19-22 Metabolomics TMS Panel EC_PF_acetate</t>
+  </si>
+  <si>
+    <t>https://anl.box.com/s/90cvb2ddpxo7kv3ek91rx1vyceko8vb9</t>
+  </si>
+  <si>
+    <t>E. coli MG1655</t>
+  </si>
+  <si>
+    <t>E. coli MG1655 with P. fluorescens</t>
+  </si>
+  <si>
+    <t>Maltose alone</t>
+  </si>
+  <si>
+    <t>Maltose and 4HB</t>
+  </si>
+  <si>
+    <t>Maltose and acetate</t>
+  </si>
+  <si>
+    <t>ODs for metabolomics</t>
+  </si>
+  <si>
+    <t>Appx. Cell ODs for Metabolomics 8-19-22 experiment</t>
+  </si>
+  <si>
+    <t>https://anl.box.com/s/s1he202yyn8tye4i104e3nc0xaoxq5a3</t>
   </si>
 </sst>
 </file>
@@ -589,26 +634,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:I12"/>
+  <dimension ref="A3:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="57.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="31.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="42.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="43.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -637,7 +681,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -657,7 +701,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -677,7 +721,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -700,7 +744,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -726,7 +770,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -752,7 +796,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -772,7 +816,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -795,7 +839,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -818,7 +862,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -842,6 +886,87 @@
       </c>
       <c r="I12" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="2">
+        <v>44855</v>
+      </c>
+      <c r="E13" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13" t="s">
+        <v>25</v>
+      </c>
+      <c r="I13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="2">
+        <v>44792</v>
+      </c>
+      <c r="E14" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" t="s">
+        <v>58</v>
+      </c>
+      <c r="H14" t="s">
+        <v>59</v>
+      </c>
+      <c r="I14" t="s">
+        <v>60</v>
+      </c>
+      <c r="J14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="2">
+        <v>44792</v>
+      </c>
+      <c r="E15" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15" t="s">
+        <v>58</v>
+      </c>
+      <c r="H15" t="s">
+        <v>59</v>
+      </c>
+      <c r="I15" t="s">
+        <v>60</v>
+      </c>
+      <c r="J15" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -855,6 +980,9 @@
     <hyperlink ref="C10" r:id="rId7"/>
     <hyperlink ref="C11" r:id="rId8"/>
     <hyperlink ref="C12" r:id="rId9"/>
+    <hyperlink ref="C13" r:id="rId10"/>
+    <hyperlink ref="C14" r:id="rId11"/>
+    <hyperlink ref="C15" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>